<commit_message>
Modificaciones a la formula de medición
</commit_message>
<xml_diff>
--- a/data/dashboards_csc.xlsx
+++ b/data/dashboards_csc.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupoalicorp-my.sharepoint.com/personal/aperalesc_alicorp_com_pe/Documents/Escritorio/github/alicorp_eda_dashboards/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_D89475C106D313929CBC3822FECCA2609D4FA6FC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C993D865-6272-4C8B-BE40-993F801CC856}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Hoja1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Hoja1!$A$1:$AB$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AB$59</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -878,7 +884,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
@@ -897,17 +903,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -920,16 +921,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -944,53 +945,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1001,10 +994,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1042,71 +1035,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1134,7 +1127,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1157,11 +1150,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1170,13 +1163,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1186,7 +1179,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1195,7 +1188,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1204,7 +1197,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1212,10 +1205,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1280,47 +1273,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="10" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="28" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1385,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1419,7 +1398,6 @@
       <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="5">
         <v>338</v>
       </c>
@@ -1490,7 +1468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="111.75">
+    <row r="3" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
@@ -1576,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="125.25">
+    <row r="4" spans="1:28" ht="125.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
@@ -1662,7 +1640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1675,7 +1653,6 @@
       <c r="D5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="1"/>
       <c r="F5" s="5">
         <v>15</v>
       </c>
@@ -1746,7 +1723,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
@@ -1756,8 +1733,6 @@
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
       <c r="F6" s="5">
         <v>7</v>
       </c>
@@ -1765,7 +1740,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="6">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="I6" s="5">
         <v>6</v>
@@ -1794,7 +1769,6 @@
       <c r="Q6" s="5">
         <v>0</v>
       </c>
-      <c r="R6" s="1"/>
       <c r="S6" s="4" t="s">
         <v>35</v>
       </c>
@@ -1826,7 +1800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="85.5">
+    <row r="7" spans="1:28" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
@@ -1912,14 +1886,13 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="125.25">
+    <row r="8" spans="1:28" ht="125.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
         <v>60</v>
       </c>
@@ -1996,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -2082,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="85.5">
+    <row r="10" spans="1:28" ht="85.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>52</v>
       </c>
@@ -2168,7 +2141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -2254,14 +2227,13 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="151.5">
+    <row r="12" spans="1:28" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="2"/>
       <c r="D12" s="4" t="s">
         <v>81</v>
       </c>
@@ -2338,14 +2310,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="45.75">
+    <row r="13" spans="1:28" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="2"/>
       <c r="D13" s="4" t="s">
         <v>86</v>
       </c>
@@ -2422,14 +2393,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="2"/>
       <c r="D14" s="4" t="s">
         <v>90</v>
       </c>
@@ -2484,7 +2454,6 @@
       <c r="U14" s="5">
         <v>687</v>
       </c>
-      <c r="V14" s="2"/>
       <c r="W14" s="5">
         <v>51</v>
       </c>
@@ -2504,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>52</v>
       </c>
@@ -2514,8 +2483,6 @@
       <c r="C15" s="5">
         <v>1</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
       <c r="F15" s="5">
         <v>80</v>
       </c>
@@ -2552,7 +2519,6 @@
       <c r="Q15" s="5">
         <v>0</v>
       </c>
-      <c r="R15" s="1"/>
       <c r="S15" s="4" t="s">
         <v>58</v>
       </c>
@@ -2562,10 +2528,6 @@
       <c r="U15" s="5">
         <v>755</v>
       </c>
-      <c r="V15" s="2"/>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
       <c r="Z15" s="5">
         <v>10</v>
       </c>
@@ -2576,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="111.75">
+    <row r="16" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
@@ -2662,7 +2624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>96</v>
       </c>
@@ -2714,7 +2676,6 @@
       <c r="Q17" s="5">
         <v>0</v>
       </c>
-      <c r="R17" s="1"/>
       <c r="S17" s="4" t="s">
         <v>101</v>
       </c>
@@ -2746,15 +2707,13 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
       <c r="E18" s="4" t="s">
         <v>104</v>
       </c>
@@ -2794,7 +2753,6 @@
       <c r="Q18" s="5">
         <v>0</v>
       </c>
-      <c r="R18" s="1"/>
       <c r="S18" s="4" t="s">
         <v>101</v>
       </c>
@@ -2826,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="111.75">
+    <row r="19" spans="1:28" ht="111.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>96</v>
       </c>
@@ -2912,14 +2870,13 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C20" s="2"/>
       <c r="D20" s="4" t="s">
         <v>114</v>
       </c>
@@ -2996,14 +2953,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="125.25">
+    <row r="21" spans="1:28" ht="125.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="2"/>
       <c r="D21" s="4" t="s">
         <v>120</v>
       </c>
@@ -3080,7 +3036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>96</v>
       </c>
@@ -3166,7 +3122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="151.5">
+    <row r="23" spans="1:28" ht="151.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>96</v>
       </c>
@@ -3252,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>96</v>
       </c>
@@ -3275,7 +3231,7 @@
         <v>11</v>
       </c>
       <c r="H24" s="6">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I24" s="5">
         <v>10</v>
@@ -3304,7 +3260,6 @@
       <c r="Q24" s="5">
         <v>0</v>
       </c>
-      <c r="R24" s="1"/>
       <c r="S24" s="4" t="s">
         <v>101</v>
       </c>
@@ -3336,14 +3291,13 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="2"/>
       <c r="D25" s="4" t="s">
         <v>98</v>
       </c>
@@ -3420,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>96</v>
       </c>
@@ -3472,7 +3426,6 @@
       <c r="Q26" s="5">
         <v>0</v>
       </c>
-      <c r="R26" s="1"/>
       <c r="S26" s="4" t="s">
         <v>101</v>
       </c>
@@ -3504,14 +3457,13 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C27" s="2"/>
       <c r="D27" s="1" t="s">
         <v>140</v>
       </c>
@@ -3588,14 +3540,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C28" s="2"/>
       <c r="D28" s="4" t="s">
         <v>140</v>
       </c>
@@ -3672,14 +3623,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C29" s="2"/>
       <c r="D29" s="4" t="s">
         <v>145</v>
       </c>
@@ -3722,7 +3672,6 @@
       <c r="Q29" s="5">
         <v>1</v>
       </c>
-      <c r="R29" s="1"/>
       <c r="S29" s="4" t="s">
         <v>101</v>
       </c>
@@ -3754,7 +3703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>96</v>
       </c>
@@ -3818,11 +3767,6 @@
       <c r="U30" s="5">
         <v>787</v>
       </c>
-      <c r="V30" s="2"/>
-      <c r="W30" s="2"/>
-      <c r="X30" s="2"/>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
       <c r="AA30" s="5">
         <v>6</v>
       </c>
@@ -3830,7 +3774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>151</v>
       </c>
@@ -3916,14 +3860,13 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>151</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="2"/>
       <c r="D32" s="4" t="s">
         <v>159</v>
       </c>
@@ -3937,7 +3880,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="6">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I32" s="5">
         <v>36</v>
@@ -4000,7 +3943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>151</v>
       </c>
@@ -4086,7 +4029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>151</v>
       </c>
@@ -4172,7 +4115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>151</v>
       </c>
@@ -4236,7 +4179,6 @@
       <c r="U35" s="5">
         <v>678</v>
       </c>
-      <c r="V35" s="2"/>
       <c r="W35" s="5">
         <v>19</v>
       </c>
@@ -4256,7 +4198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>151</v>
       </c>
@@ -4308,7 +4250,6 @@
       <c r="Q36" s="5">
         <v>0</v>
       </c>
-      <c r="R36" s="1"/>
       <c r="S36" s="4" t="s">
         <v>157</v>
       </c>
@@ -4318,11 +4259,6 @@
       <c r="U36" s="5">
         <v>764</v>
       </c>
-      <c r="V36" s="2"/>
-      <c r="W36" s="2"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
       <c r="AA36" s="5">
         <v>5</v>
       </c>
@@ -4330,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>177</v>
       </c>
@@ -4416,7 +4352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>177</v>
       </c>
@@ -4502,7 +4438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>177</v>
       </c>
@@ -4588,7 +4524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>177</v>
       </c>
@@ -4674,7 +4610,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>177</v>
       </c>
@@ -4760,7 +4696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>177</v>
       </c>
@@ -4783,7 +4719,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="6">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I42" s="5">
         <v>2</v>
@@ -4846,7 +4782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>177</v>
       </c>
@@ -4932,7 +4868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>177</v>
       </c>
@@ -4945,7 +4881,6 @@
       <c r="D44" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E44" s="1"/>
       <c r="F44" s="5">
         <v>28</v>
       </c>
@@ -5016,7 +4951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>177</v>
       </c>
@@ -5102,7 +5037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>177</v>
       </c>
@@ -5154,7 +5089,6 @@
       <c r="Q46" s="5">
         <v>0</v>
       </c>
-      <c r="R46" s="1"/>
       <c r="S46" s="4" t="s">
         <v>182</v>
       </c>
@@ -5186,7 +5120,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>177</v>
       </c>
@@ -5238,7 +5172,6 @@
       <c r="Q47" s="5">
         <v>0</v>
       </c>
-      <c r="R47" s="1"/>
       <c r="S47" s="4" t="s">
         <v>182</v>
       </c>
@@ -5270,7 +5203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>177</v>
       </c>
@@ -5356,7 +5289,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>177</v>
       </c>
@@ -5442,14 +5375,13 @@
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C50" s="2"/>
       <c r="D50" s="4" t="s">
         <v>231</v>
       </c>
@@ -5526,14 +5458,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="C51" s="2"/>
       <c r="D51" s="4" t="s">
         <v>237</v>
       </c>
@@ -5610,14 +5541,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="C52" s="2"/>
       <c r="D52" s="4" t="s">
         <v>241</v>
       </c>
@@ -5694,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>229</v>
       </c>
@@ -5780,14 +5710,13 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="C54" s="2"/>
       <c r="D54" s="4" t="s">
         <v>249</v>
       </c>
@@ -5864,14 +5793,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="C55" s="2"/>
       <c r="D55" s="4" t="s">
         <v>253</v>
       </c>
@@ -5926,9 +5854,6 @@
       <c r="U55" s="5">
         <v>723</v>
       </c>
-      <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
-      <c r="X55" s="2"/>
       <c r="Y55" s="5">
         <v>2</v>
       </c>
@@ -5942,14 +5867,13 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>229</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="C56" s="2"/>
       <c r="D56" s="4" t="s">
         <v>258</v>
       </c>
@@ -6004,9 +5928,6 @@
       <c r="U56" s="5">
         <v>730</v>
       </c>
-      <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="X56" s="2"/>
       <c r="Y56" s="5">
         <v>1</v>
       </c>
@@ -6020,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>261</v>
       </c>
@@ -6049,7 +5970,7 @@
         <v>12</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>264</v>
@@ -6106,16 +6027,13 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>261</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
       <c r="F58" s="8">
         <v>6</v>
       </c>
@@ -6152,7 +6070,6 @@
       <c r="Q58" s="8">
         <v>0</v>
       </c>
-      <c r="R58" s="1"/>
       <c r="S58" s="1" t="s">
         <v>266</v>
       </c>
@@ -6184,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:28" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>261</v>
       </c>
@@ -6271,6 +6188,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AB59" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d64a6fc3-496d-44ea-86a8-5b93f17e3566}" enabled="1" method="Standard" siteId="{3b16616d-f174-497a-a1ae-900d85106996}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>